<commit_message>
Finalizado todos os testes
</commit_message>
<xml_diff>
--- a/target/TestData.xlsx
+++ b/target/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaque.silva\Hub-workspace\ProjetoAvaliacao\target\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaque.silva\Hub-workspace\ProjetoAvaliacao_TDD\target\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EDC506-445B-4FF5-88D9-44D357813335}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCE34CF-3941-4AF4-B26C-DD96B22C7C73}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0256AA05-52C9-4FA5-99DB-EDC75ED19327}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>txtbox_UserName</t>
   </si>
@@ -125,7 +125,10 @@
     <t>isaque.silva@rsinet.com.br3</t>
   </si>
   <si>
-    <t>ISAQUEab</t>
+    <t>ISAQUEhg715</t>
+  </si>
+  <si>
+    <t>ISAQUEz1</t>
   </si>
 </sst>
 </file>
@@ -539,7 +542,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +595,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>29</v>
@@ -770,7 +773,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>